<commit_message>
completed all code and adjust
</commit_message>
<xml_diff>
--- a/TurnoverCards/翻卡礼包数值规划.xlsx
+++ b/TurnoverCards/翻卡礼包数值规划.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fotoable/Gamedev_Tools/TurnoverCards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1023F5C-78BD-564C-B647-725DB3E62591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43024062-9679-9A45-A38B-9B2FD63EDFE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="-21100" windowWidth="33600" windowHeight="18800" xr2:uid="{CEB89FA9-BF40-B240-9A33-BE725A503870}"/>
+    <workbookView xWindow="-4820" yWindow="-28300" windowWidth="49500" windowHeight="28300" xr2:uid="{CEB89FA9-BF40-B240-9A33-BE725A503870}"/>
   </bookViews>
   <sheets>
     <sheet name="奖励池" sheetId="6" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="269">
   <si>
     <t>奖励库</t>
   </si>
@@ -680,9 +680,6 @@
     <t>160~240</t>
   </si>
   <si>
-    <t>y/2</t>
-  </si>
-  <si>
     <t>奖励倍数</t>
   </si>
   <si>
@@ -692,21 +689,12 @@
     <t>x= ? y</t>
   </si>
   <si>
-    <t>则 x / y = 5 / 2 = 2.08 约定于 2</t>
-  </si>
-  <si>
-    <t>可设定在标准消费下2次低档应出1次中档</t>
-  </si>
-  <si>
     <t>2次低档消费数据</t>
   </si>
   <si>
     <t xml:space="preserve">x /y = </t>
   </si>
   <si>
-    <t>(x * 1.5+ 2.64* y + 6.42* y/2 ) / (x + y + y/2)  = 2.5</t>
-  </si>
-  <si>
     <t>高付费</t>
   </si>
   <si>
@@ -858,13 +846,49 @@
   </si>
   <si>
     <t>蝙蝠杆</t>
+  </si>
+  <si>
+    <t>因为第二次小火会直接晋升到大火</t>
+  </si>
+  <si>
+    <t>所以 y=z</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>(x * 1.5+ 2.64* y + 6.42* z ) / (x + y + z)  = 2.5</t>
+  </si>
+  <si>
+    <t>则 x / y = 5 / 2 = 4.06  约等于4</t>
+  </si>
+  <si>
+    <t>可设定在标准消费下 低档：中档： 高档 = 4:1:1</t>
+  </si>
+  <si>
+    <t>按照此比例推出节奏应为 2次无火的刷新后下一次就为小火</t>
+  </si>
+  <si>
+    <t>初步计算结果</t>
+  </si>
+  <si>
+    <t>再通过模拟器调参使得无火次数/小火次数 = 4 即可满足目标</t>
+  </si>
+  <si>
+    <t>最终参数：</t>
+  </si>
+  <si>
+    <t>再调整翻卡消耗的钻石数</t>
+  </si>
+  <si>
+    <t>再调整刷新消耗的钻石数</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -902,8 +926,14 @@
       <name val="苹方-简"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="苹方-简"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1009,6 +1039,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1143,7 +1185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1197,30 +1239,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1257,6 +1275,34 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2429,8 +2475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BDBE71F-855B-604A-8097-E2A8CAFA74DE}">
   <dimension ref="A1:X45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="131" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -2442,48 +2488,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="52" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="55" t="s">
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="57"/>
-      <c r="S1" s="58" t="s">
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
-      <c r="X1" s="60"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="52"/>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" s="31" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>110</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D2" s="31" t="s">
         <v>2</v>
@@ -2492,16 +2538,16 @@
         <v>65</v>
       </c>
       <c r="F2" s="31" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="H2" s="33" t="s">
         <v>110</v>
       </c>
       <c r="I2" s="33" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="J2" s="33" t="s">
         <v>2</v>
@@ -2510,16 +2556,16 @@
         <v>65</v>
       </c>
       <c r="L2" s="34" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="M2" s="37" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="N2" s="37" t="s">
         <v>110</v>
       </c>
       <c r="O2" s="37" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="P2" s="37" t="s">
         <v>2</v>
@@ -2528,16 +2574,16 @@
         <v>65</v>
       </c>
       <c r="R2" s="37" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="S2" s="39" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="T2" s="39" t="s">
         <v>110</v>
       </c>
       <c r="U2" s="39" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="V2" s="39" t="s">
         <v>2</v>
@@ -2546,7 +2592,7 @@
         <v>65</v>
       </c>
       <c r="X2" s="38" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:24">
@@ -2563,7 +2609,7 @@
         <v>50</v>
       </c>
       <c r="E3" s="1">
-        <v>1600</v>
+        <v>2400</v>
       </c>
       <c r="F3" s="1">
         <v>4</v>
@@ -2590,7 +2636,7 @@
         <v>43</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="O3" s="9">
         <v>10</v>
@@ -2608,7 +2654,7 @@
         <v>43</v>
       </c>
       <c r="T3" s="38" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="U3" s="38">
         <v>4</v>
@@ -2637,7 +2683,7 @@
         <v>50</v>
       </c>
       <c r="E4" s="1">
-        <v>1600</v>
+        <v>2400</v>
       </c>
       <c r="F4" s="1">
         <v>4</v>
@@ -2664,7 +2710,7 @@
         <v>42</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="O4" s="9">
         <v>100</v>
@@ -2682,7 +2728,7 @@
         <v>42</v>
       </c>
       <c r="T4" s="38" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="U4" s="38">
         <v>40</v>
@@ -2702,7 +2748,7 @@
         <v>44</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -2711,7 +2757,7 @@
         <v>50</v>
       </c>
       <c r="E5" s="1">
-        <v>1600</v>
+        <v>2400</v>
       </c>
       <c r="F5" s="1">
         <v>4</v>
@@ -2738,7 +2784,7 @@
         <v>41</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="O5" s="9">
         <v>400</v>
@@ -2756,7 +2802,7 @@
         <v>41</v>
       </c>
       <c r="T5" s="38" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="U5" s="38">
         <v>160</v>
@@ -2785,7 +2831,7 @@
         <v>50</v>
       </c>
       <c r="E6" s="1">
-        <v>1600</v>
+        <v>2400</v>
       </c>
       <c r="F6" s="1">
         <v>4</v>
@@ -2859,7 +2905,7 @@
         <v>50</v>
       </c>
       <c r="E7" s="1">
-        <v>1600</v>
+        <v>2400</v>
       </c>
       <c r="F7" s="1">
         <v>4</v>
@@ -2933,7 +2979,7 @@
         <v>50</v>
       </c>
       <c r="E8" s="1">
-        <v>1600</v>
+        <v>2400</v>
       </c>
       <c r="F8" s="1">
         <v>4</v>
@@ -3007,7 +3053,7 @@
         <v>50</v>
       </c>
       <c r="E9" s="1">
-        <v>1600</v>
+        <v>2400</v>
       </c>
       <c r="F9" s="1">
         <v>4</v>
@@ -3081,7 +3127,7 @@
         <v>50</v>
       </c>
       <c r="E10" s="1">
-        <v>1600</v>
+        <v>2400</v>
       </c>
       <c r="F10" s="1">
         <v>4</v>
@@ -3155,7 +3201,7 @@
         <v>50</v>
       </c>
       <c r="E11" s="1">
-        <v>1600</v>
+        <v>2400</v>
       </c>
       <c r="F11" s="1">
         <v>4</v>
@@ -3220,7 +3266,7 @@
         <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -3229,7 +3275,7 @@
         <v>50</v>
       </c>
       <c r="E12" s="1">
-        <v>1600</v>
+        <v>2400</v>
       </c>
       <c r="F12" s="1">
         <v>4</v>
@@ -4995,18 +5041,18 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="N5" s="43" t="s">
+      <c r="N5" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="O5" s="43"/>
-      <c r="P5" s="43"/>
-      <c r="Q5" s="43"/>
-      <c r="R5" s="43"/>
-      <c r="S5" s="43"/>
-      <c r="T5" s="43"/>
-      <c r="U5" s="43"/>
-      <c r="V5" s="43"/>
-      <c r="W5" s="43"/>
+      <c r="O5" s="55"/>
+      <c r="P5" s="55"/>
+      <c r="Q5" s="55"/>
+      <c r="R5" s="55"/>
+      <c r="S5" s="55"/>
+      <c r="T5" s="55"/>
+      <c r="U5" s="55"/>
+      <c r="V5" s="55"/>
+      <c r="W5" s="55"/>
     </row>
     <row r="7" spans="1:23">
       <c r="P7" s="10" t="s">
@@ -5023,26 +5069,26 @@
       <c r="Q8" s="10"/>
     </row>
     <row r="10" spans="1:23">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="42"/>
-      <c r="O10" s="42"/>
-      <c r="P10" s="42"/>
-      <c r="Q10" s="42"/>
-      <c r="R10" s="42"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="54"/>
     </row>
     <row r="11" spans="1:23">
       <c r="A11" s="5" t="s">
@@ -5589,18 +5635,18 @@
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="27" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B37" s="27"/>
       <c r="C37" s="26"/>
       <c r="D37" s="26" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E37" s="26"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="26" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B38" s="26"/>
       <c r="C38" s="26"/>
@@ -5609,7 +5655,7 @@
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="26" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
@@ -5625,7 +5671,7 @@
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="26" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B41" s="26"/>
       <c r="C41" s="26"/>
@@ -5647,8 +5693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC1143F6-A7C5-2A47-868E-77190750C444}">
   <dimension ref="A2:V139"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="101" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView topLeftCell="A79" zoomScale="137" workbookViewId="0">
+      <selection activeCell="N109" sqref="N109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -5994,7 +6040,7 @@
         <v>190</v>
       </c>
       <c r="S24" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="25" spans="1:22">
@@ -6005,7 +6051,7 @@
         <v>290</v>
       </c>
       <c r="L25" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M25" s="9"/>
     </row>
@@ -6048,10 +6094,10 @@
         <v>590</v>
       </c>
       <c r="H28" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I28" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L28" t="s">
         <v>122</v>
@@ -6059,6 +6105,11 @@
       <c r="M28" t="s">
         <v>125</v>
       </c>
+      <c r="N28" s="62" t="s">
+        <v>257</v>
+      </c>
+      <c r="O28" s="62"/>
+      <c r="P28" s="61"/>
       <c r="Q28" s="12" t="s">
         <v>87</v>
       </c>
@@ -6078,18 +6129,23 @@
         <v>690</v>
       </c>
       <c r="H29">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="I29">
-        <f>(1.5*H29-($N$15 + $N$18/2))/($N$12-H29)</f>
-        <v>329.05207949944918</v>
+        <f>(5-2.64-6.42)/(1.5-H29)</f>
+        <v>8.120000000000001</v>
       </c>
       <c r="L29" t="s">
         <v>123</v>
       </c>
       <c r="M29" t="s">
-        <v>201</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="N29" s="62" t="s">
+        <v>258</v>
+      </c>
+      <c r="O29" s="62"/>
+      <c r="P29" s="61"/>
       <c r="Q29" s="12" t="s">
         <v>92</v>
       </c>
@@ -6108,12 +6164,12 @@
       <c r="B30">
         <v>790</v>
       </c>
-      <c r="H30">
-        <v>1.75</v>
-      </c>
-      <c r="I30">
-        <f t="shared" ref="I30:I36" si="2">(1.5*H30-($N$15 + $N$18/2))/($N$12-H30)</f>
-        <v>12.404676384298</v>
+      <c r="H30" s="63">
+        <v>2.5</v>
+      </c>
+      <c r="I30" s="63">
+        <f t="shared" ref="I30:I36" si="2">(5-2.64-6.42)/(1.5-H30)</f>
+        <v>4.0600000000000005</v>
       </c>
       <c r="Q30" s="12" t="s">
         <v>88</v>
@@ -6134,14 +6190,14 @@
         <v>890</v>
       </c>
       <c r="H31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I31">
         <f t="shared" si="2"/>
-        <v>5.6017048329959502</v>
+        <v>2.706666666666667</v>
       </c>
       <c r="L31" t="s">
-        <v>209</v>
+        <v>260</v>
       </c>
       <c r="Q31" s="12" t="s">
         <v>89</v>
@@ -6162,23 +6218,23 @@
         <v>990</v>
       </c>
       <c r="H32">
-        <v>2.25</v>
+        <v>3.5</v>
       </c>
       <c r="I32">
         <f t="shared" si="2"/>
-        <v>3.2686201632707235</v>
+        <v>2.0300000000000002</v>
       </c>
     </row>
     <row r="33" spans="1:22">
-      <c r="H33" s="11">
-        <v>2.5</v>
-      </c>
-      <c r="I33" s="11">
+      <c r="H33">
+        <v>4</v>
+      </c>
+      <c r="I33">
         <f t="shared" si="2"/>
-        <v>2.0894105375063443</v>
+        <v>1.6240000000000001</v>
       </c>
       <c r="L33" t="s">
-        <v>205</v>
+        <v>261</v>
       </c>
       <c r="Q33" s="25" t="s">
         <v>86</v>
@@ -6198,32 +6254,35 @@
         <v>90,190,290,390,490,590,690,790,890,990</v>
       </c>
       <c r="H34">
-        <v>2.75</v>
+        <v>4.5</v>
       </c>
       <c r="I34">
         <f t="shared" si="2"/>
-        <v>1.3777782940197281</v>
+        <v>1.3533333333333335</v>
       </c>
     </row>
     <row r="35" spans="1:22">
       <c r="H35">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I35">
         <f t="shared" si="2"/>
-        <v>0.901633338503254</v>
+        <v>1.1600000000000001</v>
       </c>
       <c r="L35" t="s">
-        <v>206</v>
+        <v>262</v>
       </c>
     </row>
     <row r="36" spans="1:22">
       <c r="H36">
-        <v>3.5</v>
+        <v>5.5</v>
       </c>
       <c r="I36">
         <f t="shared" si="2"/>
-        <v>0.30450266724264341</v>
+        <v>1.0150000000000001</v>
+      </c>
+      <c r="L36" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="38" spans="1:22">
@@ -6265,13 +6324,13 @@
         <v>1</v>
       </c>
       <c r="L40" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="M40" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="N40" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="41" spans="1:22">
@@ -6282,16 +6341,16 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K41" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="L41" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="M41" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="N41" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="42" spans="1:22">
@@ -6302,16 +6361,16 @@
         <v>0.08</v>
       </c>
       <c r="K42" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="L42" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="M42" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="N42" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="43" spans="1:22">
@@ -6322,7 +6381,7 @@
         <v>0.09</v>
       </c>
       <c r="L43" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="44" spans="1:22">
@@ -6333,13 +6392,13 @@
         <v>0.1</v>
       </c>
       <c r="L44" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="M44" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="N44" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="45" spans="1:22">
@@ -6350,7 +6409,7 @@
         <v>0.11</v>
       </c>
       <c r="L45" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="46" spans="1:22">
@@ -6379,6 +6438,9 @@
       <c r="B48" s="13">
         <v>0.14000000000000001</v>
       </c>
+      <c r="N48" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="49" spans="1:15">
       <c r="A49">
@@ -6403,16 +6465,16 @@
       <c r="B51" s="13">
         <v>0.17</v>
       </c>
-      <c r="D51" s="44" t="s">
-        <v>238</v>
-      </c>
-      <c r="E51" s="44"/>
-      <c r="F51" s="44"/>
-      <c r="G51" s="44"/>
-      <c r="H51" s="44"/>
-      <c r="I51" s="44"/>
+      <c r="D51" s="56" t="s">
+        <v>234</v>
+      </c>
+      <c r="E51" s="56"/>
+      <c r="F51" s="56"/>
+      <c r="G51" s="56"/>
+      <c r="H51" s="56"/>
+      <c r="I51" s="56"/>
       <c r="L51" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="M51">
         <v>2</v>
@@ -6426,22 +6488,22 @@
         <v>0.18</v>
       </c>
       <c r="D52" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E52" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F52" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="G52" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="H52" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="I52" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="53" spans="1:15">
@@ -6452,7 +6514,7 @@
         <v>0.19</v>
       </c>
       <c r="L53" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="N53" t="s">
         <v>130</v>
@@ -6623,7 +6685,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L63" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="64" spans="1:15">
@@ -6634,7 +6696,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:15">
       <c r="A65">
         <v>26</v>
       </c>
@@ -6642,7 +6704,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:15">
       <c r="A66">
         <v>27</v>
       </c>
@@ -6650,15 +6712,18 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:15">
       <c r="A67">
         <v>28</v>
       </c>
       <c r="B67" s="13">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
+      <c r="L67" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15">
       <c r="A68">
         <v>29</v>
       </c>
@@ -6666,55 +6731,91 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:15">
       <c r="A69">
         <v>30</v>
       </c>
       <c r="B69" s="13">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="70" spans="1:2">
+      <c r="L69" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15">
       <c r="A70">
         <v>31</v>
       </c>
       <c r="B70" s="13">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="71" spans="1:2">
+      <c r="L70" t="s">
+        <v>204</v>
+      </c>
+      <c r="N70" t="s">
+        <v>130</v>
+      </c>
+      <c r="O70" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15">
       <c r="A71">
         <v>32</v>
       </c>
       <c r="B71" s="13">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
+      <c r="L71" t="s">
+        <v>128</v>
+      </c>
+      <c r="O71">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15">
       <c r="A72">
         <v>33</v>
       </c>
       <c r="B72" s="13">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="73" spans="1:2">
+      <c r="L72" t="s">
+        <v>93</v>
+      </c>
+      <c r="O72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15">
       <c r="A73">
         <v>34</v>
       </c>
       <c r="B73" s="13">
         <v>0.39</v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
+      <c r="L73" t="s">
+        <v>126</v>
+      </c>
+      <c r="O73">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15">
       <c r="A74">
         <v>35</v>
       </c>
       <c r="B74" s="13">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
+      <c r="L74" t="s">
+        <v>127</v>
+      </c>
+      <c r="O74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15">
       <c r="A75">
         <v>36</v>
       </c>
@@ -6722,15 +6823,18 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:15">
       <c r="A76">
         <v>37</v>
       </c>
       <c r="B76" s="13">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="77" spans="1:2">
+      <c r="L76" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15">
       <c r="A77">
         <v>38</v>
       </c>
@@ -6738,15 +6842,21 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:15">
       <c r="A78">
         <v>39</v>
       </c>
       <c r="B78" s="13">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="79" spans="1:2">
+      <c r="L78" t="s">
+        <v>129</v>
+      </c>
+      <c r="O78">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15">
       <c r="A79" s="23">
         <v>40</v>
       </c>
@@ -6754,7 +6864,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:15">
       <c r="A80">
         <v>41</v>
       </c>
@@ -6762,95 +6872,199 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:14">
       <c r="A81">
         <v>42</v>
       </c>
       <c r="B81" s="13">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="82" spans="1:2">
+      <c r="L81" s="64" t="s">
+        <v>267</v>
+      </c>
+      <c r="M81" s="64"/>
+      <c r="N81" s="64"/>
+    </row>
+    <row r="82" spans="1:14">
       <c r="A82">
         <v>43</v>
       </c>
       <c r="B82" s="13">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="83" spans="1:2">
+      <c r="L82" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="M82" s="64" t="s">
+        <v>63</v>
+      </c>
+      <c r="N82" s="64" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14">
       <c r="A83">
         <v>44</v>
       </c>
       <c r="B83" s="13">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="84" spans="1:2">
+      <c r="L83" s="64">
+        <v>1</v>
+      </c>
+      <c r="M83" s="64">
+        <v>60</v>
+      </c>
+      <c r="N83" s="64">
+        <f>SUM($B$3:M83)</f>
+        <v>67575.719000000012</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14">
       <c r="A84">
         <v>45</v>
       </c>
       <c r="B84" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="85" spans="1:2">
+      <c r="L84" s="64">
+        <v>2</v>
+      </c>
+      <c r="M84" s="64">
+        <v>100</v>
+      </c>
+      <c r="N84" s="64">
+        <f>SUM($B$3:M84)</f>
+        <v>67678.219000000012</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14">
       <c r="A85">
         <v>46</v>
       </c>
       <c r="B85" s="13">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="86" spans="1:2">
+      <c r="L85" s="64">
+        <v>3</v>
+      </c>
+      <c r="M85" s="64">
+        <v>160</v>
+      </c>
+      <c r="N85" s="64">
+        <f>SUM($B$3:M85)</f>
+        <v>67841.729000000007</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14">
       <c r="A86">
         <v>47</v>
       </c>
       <c r="B86" s="13">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="87" spans="1:2">
+      <c r="L86" s="64">
+        <v>4</v>
+      </c>
+      <c r="M86" s="64">
+        <v>260</v>
+      </c>
+      <c r="N86" s="64">
+        <f>SUM($B$3:M86)</f>
+        <v>68106.249000000011</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14">
       <c r="A87">
         <v>48</v>
       </c>
       <c r="B87" s="13">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="88" spans="1:2">
+      <c r="L87" s="64">
+        <v>5</v>
+      </c>
+      <c r="M87" s="64">
+        <v>360</v>
+      </c>
+      <c r="N87" s="64">
+        <f>SUM($B$3:M87)</f>
+        <v>68471.77900000001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14">
       <c r="A88">
         <v>49</v>
       </c>
       <c r="B88" s="13">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="89" spans="1:2">
+      <c r="L88" s="64">
+        <v>6</v>
+      </c>
+      <c r="M88" s="64">
+        <v>460</v>
+      </c>
+      <c r="N88" s="64">
+        <f>SUM($B$3:M88)</f>
+        <v>68938.319000000003</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14">
       <c r="A89">
         <v>50</v>
       </c>
       <c r="B89" s="13">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="90" spans="1:2">
+      <c r="L89" s="64">
+        <v>7</v>
+      </c>
+      <c r="M89" s="64">
+        <v>560</v>
+      </c>
+      <c r="N89" s="64">
+        <f>SUM($B$3:M89)</f>
+        <v>69505.869000000006</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14">
       <c r="A90">
         <v>51</v>
       </c>
       <c r="B90" s="13">
         <v>0.56000000000000005</v>
       </c>
-    </row>
-    <row r="91" spans="1:2">
+      <c r="L90" s="64">
+        <v>8</v>
+      </c>
+      <c r="M90" s="64">
+        <v>660</v>
+      </c>
+      <c r="N90" s="64">
+        <f>SUM($B$3:M90)</f>
+        <v>70174.429000000004</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14">
       <c r="A91">
         <v>52</v>
       </c>
       <c r="B91" s="13">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="92" spans="1:2">
+      <c r="L91" s="64">
+        <v>9</v>
+      </c>
+      <c r="M91" s="64">
+        <v>760</v>
+      </c>
+      <c r="N91" s="64">
+        <f>SUM($B$3:M91)</f>
+        <v>70943.999000000011</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14">
       <c r="A92">
         <v>53</v>
       </c>
@@ -6858,15 +7072,19 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:14">
       <c r="A93">
         <v>54</v>
       </c>
       <c r="B93" s="13">
         <v>0.59</v>
       </c>
-    </row>
-    <row r="94" spans="1:2">
+      <c r="M93" t="str">
+        <f>_xlfn.TEXTJOIN(",",FALSE,M83:M91)</f>
+        <v>60,100,160,260,360,460,560,660,760</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14">
       <c r="A94">
         <v>55</v>
       </c>
@@ -6874,95 +7092,170 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:14">
       <c r="A95">
         <v>56</v>
       </c>
       <c r="B95" s="13">
         <v>0.61</v>
       </c>
-    </row>
-    <row r="96" spans="1:2">
+      <c r="L95" s="64" t="s">
+        <v>268</v>
+      </c>
+      <c r="M95" s="64"/>
+      <c r="N95" s="64"/>
+    </row>
+    <row r="96" spans="1:14">
       <c r="A96">
         <v>57</v>
       </c>
       <c r="B96" s="13">
         <v>0.62</v>
       </c>
-    </row>
-    <row r="97" spans="1:2">
+      <c r="L96" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="M96" s="64" t="s">
+        <v>62</v>
+      </c>
+      <c r="N96" s="64"/>
+    </row>
+    <row r="97" spans="1:14">
       <c r="A97">
         <v>58</v>
       </c>
       <c r="B97" s="13">
         <v>0.63</v>
       </c>
-    </row>
-    <row r="98" spans="1:2">
+      <c r="L97" s="64">
+        <v>1</v>
+      </c>
+      <c r="M97" s="64">
+        <v>60</v>
+      </c>
+      <c r="N97" s="64"/>
+    </row>
+    <row r="98" spans="1:14">
       <c r="A98">
         <v>59</v>
       </c>
       <c r="B98" s="13">
         <v>0.64</v>
       </c>
-    </row>
-    <row r="99" spans="1:2">
+      <c r="L98" s="64">
+        <v>2</v>
+      </c>
+      <c r="M98" s="64">
+        <v>100</v>
+      </c>
+      <c r="N98" s="64"/>
+    </row>
+    <row r="99" spans="1:14">
       <c r="A99">
         <v>60</v>
       </c>
       <c r="B99" s="13">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="100" spans="1:2">
+      <c r="L99" s="64">
+        <v>3</v>
+      </c>
+      <c r="M99" s="64">
+        <v>160</v>
+      </c>
+      <c r="N99" s="64"/>
+    </row>
+    <row r="100" spans="1:14">
       <c r="A100">
         <v>61</v>
       </c>
       <c r="B100" s="13">
         <v>0.66</v>
       </c>
-    </row>
-    <row r="101" spans="1:2">
+      <c r="L100" s="64">
+        <v>4</v>
+      </c>
+      <c r="M100" s="64">
+        <v>260</v>
+      </c>
+      <c r="N100" s="64"/>
+    </row>
+    <row r="101" spans="1:14">
       <c r="A101">
         <v>62</v>
       </c>
       <c r="B101" s="13">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="102" spans="1:2">
+      <c r="L101" s="64">
+        <v>5</v>
+      </c>
+      <c r="M101" s="64">
+        <v>360</v>
+      </c>
+      <c r="N101" s="64"/>
+    </row>
+    <row r="102" spans="1:14">
       <c r="A102">
         <v>63</v>
       </c>
       <c r="B102" s="13">
         <v>0.68</v>
       </c>
-    </row>
-    <row r="103" spans="1:2">
+      <c r="L102" s="64">
+        <v>6</v>
+      </c>
+      <c r="M102" s="64">
+        <v>460</v>
+      </c>
+      <c r="N102" s="64"/>
+    </row>
+    <row r="103" spans="1:14">
       <c r="A103">
         <v>64</v>
       </c>
       <c r="B103" s="13">
         <v>0.69</v>
       </c>
-    </row>
-    <row r="104" spans="1:2">
+      <c r="L103" s="64">
+        <v>7</v>
+      </c>
+      <c r="M103" s="64">
+        <v>560</v>
+      </c>
+      <c r="N103" s="64"/>
+    </row>
+    <row r="104" spans="1:14">
       <c r="A104">
         <v>65</v>
       </c>
       <c r="B104" s="13">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="105" spans="1:2">
+      <c r="L104" s="64">
+        <v>8</v>
+      </c>
+      <c r="M104" s="64">
+        <v>660</v>
+      </c>
+      <c r="N104" s="64"/>
+    </row>
+    <row r="105" spans="1:14">
       <c r="A105">
         <v>66</v>
       </c>
       <c r="B105" s="13">
         <v>0.71</v>
       </c>
-    </row>
-    <row r="106" spans="1:2">
+      <c r="L105" s="64">
+        <v>9</v>
+      </c>
+      <c r="M105" s="64">
+        <v>760</v>
+      </c>
+      <c r="N105" s="64"/>
+    </row>
+    <row r="106" spans="1:14">
       <c r="A106">
         <v>67</v>
       </c>
@@ -6970,7 +7263,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:14">
       <c r="A107">
         <v>68</v>
       </c>
@@ -6978,7 +7271,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:14">
       <c r="A108">
         <v>69</v>
       </c>
@@ -6986,7 +7279,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:14">
       <c r="A109">
         <v>70</v>
       </c>
@@ -6994,7 +7287,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:14">
       <c r="A110">
         <v>71</v>
       </c>
@@ -7002,7 +7295,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:14">
       <c r="A111">
         <v>72</v>
       </c>
@@ -7010,7 +7303,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:14">
       <c r="A112">
         <v>73</v>
       </c>
@@ -7244,7 +7537,7 @@
         <v>134</v>
       </c>
       <c r="M1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -7252,7 +7545,7 @@
         <v>135</v>
       </c>
       <c r="M3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="N3" t="s">
         <v>56</v>
@@ -7261,13 +7554,13 @@
     <row r="4" spans="1:16">
       <c r="A4" s="12"/>
       <c r="M4" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="N4" t="s">
         <v>55</v>
       </c>
       <c r="O4" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -7278,13 +7571,13 @@
         <v>141</v>
       </c>
       <c r="M5" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="N5" t="s">
         <v>57</v>
       </c>
       <c r="O5" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -7305,7 +7598,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="M9" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -7313,13 +7606,13 @@
         <v>136</v>
       </c>
       <c r="M10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="N10" t="s">
+        <v>214</v>
+      </c>
+      <c r="P10" t="s">
         <v>218</v>
-      </c>
-      <c r="P10" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -7330,13 +7623,13 @@
         <v>3</v>
       </c>
       <c r="M11" t="s">
+        <v>215</v>
+      </c>
+      <c r="N11" t="s">
+        <v>216</v>
+      </c>
+      <c r="P11" t="s">
         <v>219</v>
-      </c>
-      <c r="N11" t="s">
-        <v>220</v>
-      </c>
-      <c r="P11" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -7347,13 +7640,13 @@
         <v>1</v>
       </c>
       <c r="M12" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="N12" t="s">
+        <v>216</v>
+      </c>
+      <c r="P12" t="s">
         <v>220</v>
-      </c>
-      <c r="P12" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -7485,11 +7778,11 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="47"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="59"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="14" t="s">
@@ -7642,11 +7935,11 @@
       <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="48"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="60"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="14" t="s">

</xml_diff>